<commit_message>
tweaked schedule so that the practical topics match the chapter headings
</commit_message>
<xml_diff>
--- a/BB852_Schedule.xlsx
+++ b/BB852_Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jones/Dropbox/_SDU_Teaching/BB852/Course Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59275D87-7865-E243-9BD6-61D4BE06A6F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD7D10A-E043-7142-9EEC-35459E9E4C99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="27220" xr2:uid="{CCA45BD5-8A90-4848-8BF8-FC958BC91D48}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="59">
   <si>
     <t>Topic</t>
   </si>
@@ -89,18 +89,12 @@
     <t>Data management</t>
   </si>
   <si>
-    <t>Using dplyr</t>
-  </si>
-  <si>
     <t>Data visualistion</t>
   </si>
   <si>
     <t>Data handling</t>
   </si>
   <si>
-    <t>Data visualisation with ggplot2.</t>
-  </si>
-  <si>
     <t>Summary statistics, distributions and probability</t>
   </si>
   <si>
@@ -128,9 +122,6 @@
     <t>t-tests</t>
   </si>
   <si>
-    <t>Data wrangling in R</t>
-  </si>
-  <si>
     <t>Using ggplot</t>
   </si>
   <si>
@@ -204,6 +195,21 @@
   </si>
   <si>
     <t>Two-way anova in R</t>
+  </si>
+  <si>
+    <t>Data wrangling with dplyr</t>
+  </si>
+  <si>
+    <t>Exercise: Wrangling the Amniote Life History Database</t>
+  </si>
+  <si>
+    <t>Combining data sets</t>
+  </si>
+  <si>
+    <t>Exercise: Temperature effects on egg laying dates</t>
+  </si>
+  <si>
+    <t>Data visualisation with ggplot2</t>
   </si>
 </sst>
 </file>
@@ -567,7 +573,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -577,19 +583,19 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
         <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F1" t="s">
         <v>15</v>
@@ -601,7 +607,7 @@
         <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J1" t="s">
         <v>9</v>
@@ -680,10 +686,10 @@
         <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>1</v>
@@ -712,10 +718,10 @@
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -732,7 +738,7 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
@@ -761,13 +767,13 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="H7">
         <v>3</v>
@@ -790,7 +796,7 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
         <v>5</v>
@@ -799,13 +805,13 @@
         <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I8">
         <v>3</v>
       </c>
       <c r="J8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -822,16 +828,16 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
         <v>3</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I9">
         <v>3</v>
@@ -851,16 +857,16 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="H10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I10">
         <v>3</v>
@@ -880,16 +886,16 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
         <v>3</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="H11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I11">
         <v>3</v>
@@ -909,13 +915,13 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
         <v>5</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="H12">
         <v>5</v>
@@ -938,13 +944,13 @@
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
         <v>3</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H13">
         <v>5</v>
@@ -967,13 +973,13 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H14">
         <v>6</v>
@@ -996,13 +1002,13 @@
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" t="s">
         <v>3</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H15">
         <v>6</v>
@@ -1025,13 +1031,13 @@
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F16" t="s">
         <v>3</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H16">
         <v>7</v>
@@ -1054,13 +1060,13 @@
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F17" t="s">
         <v>3</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H17">
         <v>7</v>
@@ -1069,7 +1075,7 @@
         <v>8</v>
       </c>
       <c r="J17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1086,7 +1092,7 @@
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F18" t="s">
         <v>5</v>
@@ -1112,7 +1118,7 @@
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F19" t="s">
         <v>3</v>
@@ -1138,7 +1144,7 @@
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F20" t="s">
         <v>3</v>
@@ -1164,7 +1170,7 @@
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F21" t="s">
         <v>3</v>
@@ -1190,13 +1196,13 @@
         <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F22" t="s">
         <v>5</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H22">
         <v>9</v>
@@ -1219,13 +1225,13 @@
         <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F23" t="s">
         <v>3</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H23">
         <v>9</v>
@@ -1245,13 +1251,13 @@
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F24" t="s">
         <v>5</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H24">
         <v>10</v>
@@ -1274,13 +1280,13 @@
         <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F25" t="s">
         <v>3</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H25">
         <v>10</v>
@@ -1300,13 +1306,13 @@
         <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F26" t="s">
         <v>5</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H26">
         <v>11</v>
@@ -1329,13 +1335,13 @@
         <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F27" t="s">
         <v>3</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H27">
         <v>11</v>
@@ -1355,13 +1361,13 @@
         <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F28" t="s">
         <v>5</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H28">
         <v>12</v>
@@ -1384,13 +1390,13 @@
         <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F29" t="s">
         <v>3</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H29">
         <v>12</v>
@@ -1410,13 +1416,13 @@
         <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F30" t="s">
         <v>5</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H30">
         <v>12</v>
@@ -1436,13 +1442,13 @@
         <v>30</v>
       </c>
       <c r="E31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F31" t="s">
         <v>3</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H31">
         <v>13</v>
@@ -1462,13 +1468,13 @@
         <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F32" t="s">
         <v>5</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H32">
         <v>14</v>
@@ -1491,13 +1497,13 @@
         <v>32</v>
       </c>
       <c r="E33" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F33" t="s">
         <v>3</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H33">
         <v>14</v>
@@ -1517,13 +1523,13 @@
         <v>33</v>
       </c>
       <c r="E34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F34" t="s">
         <v>5</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H34">
         <v>15</v>
@@ -1546,13 +1552,13 @@
         <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F35" t="s">
         <v>3</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H35">
         <v>15</v>
@@ -1572,13 +1578,13 @@
         <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F36" t="s">
         <v>5</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H36">
         <v>16</v>
@@ -1598,13 +1604,13 @@
         <v>36</v>
       </c>
       <c r="E37" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F37" t="s">
         <v>3</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H37">
         <v>16</v>
@@ -1624,13 +1630,13 @@
         <v>37</v>
       </c>
       <c r="E38" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F38" t="s">
         <v>3</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1647,13 +1653,13 @@
         <v>38</v>
       </c>
       <c r="E39" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F39" t="s">
         <v>3</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1670,13 +1676,13 @@
         <v>39</v>
       </c>
       <c r="E40" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F40" t="s">
         <v>3</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1693,13 +1699,13 @@
         <v>40</v>
       </c>
       <c r="E41" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F41" t="s">
         <v>3</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1716,13 +1722,13 @@
         <v>41</v>
       </c>
       <c r="E42" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F42" t="s">
         <v>3</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1739,13 +1745,13 @@
         <v>42</v>
       </c>
       <c r="E43" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F43" t="s">
         <v>3</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1762,13 +1768,13 @@
         <v>43</v>
       </c>
       <c r="E44" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F44" t="s">
         <v>5</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1785,13 +1791,13 @@
         <v>44</v>
       </c>
       <c r="E45" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F45" t="s">
         <v>5</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added stuff about pivot
</commit_message>
<xml_diff>
--- a/BB852_Schedule.xlsx
+++ b/BB852_Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jones/Dropbox/_SDU_Teaching/BB852/Course Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD7D10A-E043-7142-9EEC-35459E9E4C99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47752491-0F95-D242-90D0-42D94E8E5129}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="27220" xr2:uid="{CCA45BD5-8A90-4848-8BF8-FC958BC91D48}"/>
   </bookViews>
@@ -573,7 +573,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -799,10 +799,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="H8" t="s">
         <v>23</v>
@@ -860,10 +860,10 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>56</v>
+        <v>5</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="H10" t="s">
         <v>23</v>
@@ -892,7 +892,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H11" t="s">
         <v>23</v>
@@ -915,13 +915,13 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>58</v>
+        <v>3</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="H12">
         <v>5</v>
@@ -947,10 +947,10 @@
         <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>29</v>
+        <v>5</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="H13">
         <v>5</v>
@@ -976,10 +976,10 @@
         <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>20</v>
+        <v>3</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="H14">
         <v>6</v>
@@ -1005,10 +1005,10 @@
         <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>30</v>
+        <v>5</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="H15">
         <v>6</v>
@@ -1036,8 +1036,8 @@
       <c r="F16" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>21</v>
+      <c r="G16" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="H16">
         <v>7</v>
@@ -1092,13 +1092,13 @@
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="H18">
         <v>8</v>
@@ -1121,10 +1121,10 @@
         <v>27</v>
       </c>
       <c r="F19" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H19">
         <v>8</v>
@@ -1199,10 +1199,10 @@
         <v>27</v>
       </c>
       <c r="F22" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="H22">
         <v>9</v>
@@ -1228,10 +1228,10 @@
         <v>27</v>
       </c>
       <c r="F23" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H23">
         <v>9</v>
@@ -1254,10 +1254,10 @@
         <v>27</v>
       </c>
       <c r="F24" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H24">
         <v>10</v>
@@ -1283,10 +1283,10 @@
         <v>27</v>
       </c>
       <c r="F25" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H25">
         <v>10</v>
@@ -1309,10 +1309,10 @@
         <v>27</v>
       </c>
       <c r="F26" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H26">
         <v>11</v>
@@ -1338,10 +1338,10 @@
         <v>27</v>
       </c>
       <c r="F27" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H27">
         <v>11</v>
@@ -1364,10 +1364,10 @@
         <v>27</v>
       </c>
       <c r="F28" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H28">
         <v>12</v>
@@ -1393,10 +1393,10 @@
         <v>27</v>
       </c>
       <c r="F29" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="H29">
         <v>12</v>
@@ -1419,10 +1419,10 @@
         <v>27</v>
       </c>
       <c r="F30" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="H30">
         <v>12</v>
@@ -1445,10 +1445,10 @@
         <v>27</v>
       </c>
       <c r="F31" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="H31">
         <v>13</v>
@@ -1471,10 +1471,10 @@
         <v>27</v>
       </c>
       <c r="F32" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="H32">
         <v>14</v>
@@ -1500,10 +1500,10 @@
         <v>27</v>
       </c>
       <c r="F33" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H33">
         <v>14</v>
@@ -1526,10 +1526,10 @@
         <v>27</v>
       </c>
       <c r="F34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H34">
         <v>15</v>
@@ -1555,10 +1555,10 @@
         <v>27</v>
       </c>
       <c r="F35" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H35">
         <v>15</v>
@@ -1581,10 +1581,10 @@
         <v>27</v>
       </c>
       <c r="F36" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H36">
         <v>16</v>
@@ -1607,10 +1607,10 @@
         <v>27</v>
       </c>
       <c r="F37" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H37">
         <v>16</v>
@@ -1630,13 +1630,13 @@
         <v>37</v>
       </c>
       <c r="E38" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="F38" t="s">
         <v>3</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:9">

</xml_diff>

<commit_message>
Modified schedule.Rmd to add personal calendars
</commit_message>
<xml_diff>
--- a/BB852_Schedule.xlsx
+++ b/BB852_Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jones/Dropbox/_SDU_Teaching/BB852/Course Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108FF6B5-34AE-EC46-A8F1-BA6578D32A3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1FE8D9-0788-754A-992C-3C731F0D074B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="27220" xr2:uid="{CCA45BD5-8A90-4848-8BF8-FC958BC91D48}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="61">
   <si>
     <t>Topic</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t>Data visualisation with ggplot2</t>
+  </si>
+  <si>
+    <t>Instructor</t>
+  </si>
+  <si>
+    <t>OJ</t>
   </si>
 </sst>
 </file>
@@ -570,18 +576,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C11A616-6116-174C-ABC2-888311E75E63}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="7" max="7" width="46.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -603,17 +610,20 @@
       <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
-        <v>11</v>
+      <c r="H1" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>2</v>
       </c>
@@ -635,9 +645,12 @@
       <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="H2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>2</v>
       </c>
@@ -659,11 +672,14 @@
       <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>4</v>
       </c>
@@ -685,17 +701,20 @@
       <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H4" t="s">
-        <v>24</v>
+      <c r="H4" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="I4" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>4</v>
       </c>
@@ -717,14 +736,17 @@
       <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H5" t="s">
-        <v>24</v>
+      <c r="H5" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="I5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>9</v>
       </c>
@@ -746,14 +768,17 @@
       <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H6">
-        <v>3</v>
+      <c r="H6" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="I6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="J6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>9</v>
       </c>
@@ -775,14 +800,17 @@
       <c r="G7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H7">
-        <v>3</v>
+      <c r="H7" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="I7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="J7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>11</v>
       </c>
@@ -804,17 +832,20 @@
       <c r="G8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" t="s">
         <v>23</v>
       </c>
-      <c r="I8">
-        <v>3</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="K8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>11</v>
       </c>
@@ -836,14 +867,17 @@
       <c r="G9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" t="s">
         <v>23</v>
       </c>
-      <c r="I9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="J9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>15</v>
       </c>
@@ -865,14 +899,17 @@
       <c r="G10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" t="s">
         <v>23</v>
       </c>
-      <c r="I10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="J10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>15</v>
       </c>
@@ -894,14 +931,17 @@
       <c r="G11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" t="s">
         <v>23</v>
       </c>
-      <c r="I11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="J11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>18</v>
       </c>
@@ -923,14 +963,17 @@
       <c r="G12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H12">
-        <v>5</v>
+      <c r="H12" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>18</v>
       </c>
@@ -952,14 +995,17 @@
       <c r="G13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H13">
-        <v>5</v>
+      <c r="H13" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="I13">
+        <v>5</v>
+      </c>
+      <c r="J13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>22</v>
       </c>
@@ -981,14 +1027,17 @@
       <c r="G14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14">
         <v>6</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>22</v>
       </c>
@@ -1010,14 +1059,17 @@
       <c r="G15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15">
         <v>6</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>24</v>
       </c>
@@ -1039,14 +1091,17 @@
       <c r="G16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16">
         <v>7</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>24</v>
       </c>
@@ -1068,17 +1123,20 @@
       <c r="G17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17">
         <v>7</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>8</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>29</v>
       </c>
@@ -1100,11 +1158,14 @@
       <c r="G18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>29</v>
       </c>
@@ -1126,11 +1187,14 @@
       <c r="G19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1152,11 +1216,14 @@
       <c r="G20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1178,11 +1245,14 @@
       <c r="G21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I21">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>7</v>
       </c>
@@ -1204,14 +1274,17 @@
       <c r="G22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H22">
-        <v>9</v>
+      <c r="H22" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="I22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+        <v>9</v>
+      </c>
+      <c r="J22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>7</v>
       </c>
@@ -1233,11 +1306,14 @@
       <c r="G23" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H23">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="H23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>8</v>
       </c>
@@ -1259,14 +1335,17 @@
       <c r="G24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24">
         <v>10</v>
       </c>
-      <c r="I24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="J24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>8</v>
       </c>
@@ -1288,11 +1367,14 @@
       <c r="G25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I25">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>26</v>
       </c>
@@ -1314,14 +1396,17 @@
       <c r="G26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H26">
-        <v>11</v>
+      <c r="H26" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="I26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+        <v>11</v>
+      </c>
+      <c r="J26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1343,11 +1428,14 @@
       <c r="G27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H27">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="H27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>29</v>
       </c>
@@ -1369,14 +1457,17 @@
       <c r="G28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I28">
         <v>12</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>29</v>
       </c>
@@ -1398,11 +1489,14 @@
       <c r="G29" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I29">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1424,11 +1518,14 @@
       <c r="G30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I30">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:11">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1450,11 +1547,14 @@
       <c r="G31" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I31">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:11">
       <c r="A32">
         <v>6</v>
       </c>
@@ -1476,14 +1576,17 @@
       <c r="G32" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I32">
         <v>14</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>6</v>
       </c>
@@ -1505,11 +1608,14 @@
       <c r="G33" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I33">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>11</v>
       </c>
@@ -1531,14 +1637,17 @@
       <c r="G34" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I34">
         <v>15</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>11</v>
       </c>
@@ -1560,11 +1669,14 @@
       <c r="G35" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I35">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>13</v>
       </c>
@@ -1586,11 +1698,14 @@
       <c r="G36" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I36">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>13</v>
       </c>
@@ -1612,11 +1727,14 @@
       <c r="G37" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I37">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>17</v>
       </c>
@@ -1638,8 +1756,11 @@
       <c r="G38" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="H38" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>17</v>
       </c>
@@ -1661,8 +1782,11 @@
       <c r="G39" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="H39" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>19</v>
       </c>
@@ -1684,8 +1808,11 @@
       <c r="G40" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="H40" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>19</v>
       </c>
@@ -1707,8 +1834,11 @@
       <c r="G41" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="H41" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>25</v>
       </c>
@@ -1730,8 +1860,11 @@
       <c r="G42" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="H42" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>25</v>
       </c>
@@ -1753,8 +1886,11 @@
       <c r="G43" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="H43" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>26</v>
       </c>
@@ -1776,8 +1912,11 @@
       <c r="G44" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="H44" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>26</v>
       </c>
@@ -1798,6 +1937,9 @@
       </c>
       <c r="G45" s="2" t="s">
         <v>47</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added section about paths and projects
</commit_message>
<xml_diff>
--- a/BB852_Schedule.xlsx
+++ b/BB852_Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jones/Dropbox/_SDU_Teaching/BB852/BB852_Book/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jones/Dropbox/_SDU_Teaching/BB852/Course Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE2622C-5D69-1D4C-B795-254232FD9402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EFC879-BE6D-A146-A058-5AB7BDBEEACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="27220" xr2:uid="{CCA45BD5-8A90-4848-8BF8-FC958BC91D48}"/>
   </bookViews>
@@ -116,6 +116,9 @@
     <t>Using ggplot</t>
   </si>
   <si>
+    <t>t-tests in R</t>
+  </si>
+  <si>
     <t>ANOVA</t>
   </si>
   <si>
@@ -200,6 +203,9 @@
     <t>Randomisation tests in R</t>
   </si>
   <si>
+    <t>Paired randomisation tests</t>
+  </si>
+  <si>
     <t>Getting acquainted with R; An R refresher</t>
   </si>
   <si>
@@ -207,12 +213,6 @@
   </si>
   <si>
     <t>Probability and distributions in R; Exercise: Virtual dice</t>
-  </si>
-  <si>
-    <t>t-tests in R; Two t-test exercises</t>
-  </si>
-  <si>
-    <t>Paired randomisation tests in R</t>
   </si>
 </sst>
 </file>
@@ -590,7 +590,7 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
         <v>13</v>
@@ -599,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F1" t="s">
         <v>9</v>
@@ -625,7 +625,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F2" s="3"/>
     </row>
@@ -643,7 +643,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>8</v>
@@ -660,10 +660,10 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
         <v>21</v>
@@ -686,10 +686,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
         <v>21</v>
@@ -712,7 +712,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -732,10 +732,10 @@
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -758,7 +758,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
@@ -781,10 +781,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
@@ -804,10 +804,10 @@
         <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
@@ -827,10 +827,10 @@
         <v>3</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
@@ -850,10 +850,10 @@
         <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F12">
         <v>5</v>
@@ -876,7 +876,7 @@
         <v>26</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F13">
         <v>5</v>
@@ -899,7 +899,7 @@
         <v>17</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F14">
         <v>6</v>
@@ -919,10 +919,10 @@
         <v>3</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F15">
         <v>6</v>
@@ -945,7 +945,7 @@
         <v>18</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F16">
         <v>7</v>
@@ -968,7 +968,7 @@
         <v>18</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F17">
         <v>7</v>
@@ -994,7 +994,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F18">
         <v>8</v>
@@ -1011,10 +1011,10 @@
         <v>3</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F19">
         <v>8</v>
@@ -1031,10 +1031,10 @@
         <v>3</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F20">
         <v>8</v>
@@ -1051,10 +1051,10 @@
         <v>3</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F21">
         <v>8</v>
@@ -1074,7 +1074,7 @@
         <v>25</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F22">
         <v>9</v>
@@ -1094,10 +1094,10 @@
         <v>3</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F23">
         <v>9</v>
@@ -1114,10 +1114,10 @@
         <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F24">
         <v>10</v>
@@ -1137,10 +1137,10 @@
         <v>3</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F25">
         <v>10</v>
@@ -1157,10 +1157,10 @@
         <v>4</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F26">
         <v>11</v>
@@ -1180,10 +1180,10 @@
         <v>3</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F27">
         <v>11</v>
@@ -1200,10 +1200,10 @@
         <v>4</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F28">
         <v>12</v>
@@ -1223,10 +1223,10 @@
         <v>3</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F29">
         <v>12</v>
@@ -1243,10 +1243,10 @@
         <v>4</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F30">
         <v>12</v>
@@ -1263,10 +1263,10 @@
         <v>3</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F31">
         <v>13</v>
@@ -1283,10 +1283,10 @@
         <v>4</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F32">
         <v>14</v>
@@ -1306,10 +1306,10 @@
         <v>3</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F33">
         <v>14</v>
@@ -1326,10 +1326,10 @@
         <v>4</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F34">
         <v>15</v>
@@ -1349,10 +1349,10 @@
         <v>3</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F35">
         <v>15</v>
@@ -1369,10 +1369,10 @@
         <v>4</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F36">
         <v>16</v>
@@ -1389,10 +1389,10 @@
         <v>3</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F37">
         <v>16</v>
@@ -1403,16 +1403,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1420,16 +1420,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
         <v>3</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1437,16 +1437,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C40" t="s">
         <v>3</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1454,16 +1454,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C41" t="s">
         <v>3</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1471,16 +1471,16 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C42" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1488,16 +1488,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C43" t="s">
         <v>3</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1505,16 +1505,16 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C44" t="s">
         <v>4</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1522,16 +1522,16 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
         <v>4</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Error fixes and rebuild
</commit_message>
<xml_diff>
--- a/BB852_Schedule.xlsx
+++ b/BB852_Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jones/Dropbox/_SDU_Teaching/BB852/Course Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EFC879-BE6D-A146-A058-5AB7BDBEEACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339FC4AB-0F87-214A-B799-0069DEE44F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="27220" xr2:uid="{CCA45BD5-8A90-4848-8BF8-FC958BC91D48}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{CCA45BD5-8A90-4848-8BF8-FC958BC91D48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="53">
   <si>
     <t>Topic</t>
   </si>
   <si>
-    <t>Petchey, O., Beckerman, A., &amp; Childs, D. (2009). Shock and Awe by Statistical Software - Why R? Bulletin of the British Ecological Society, 40(4), 55–58.</t>
-  </si>
-  <si>
     <t>Randomisation tests</t>
   </si>
   <si>
@@ -56,15 +53,6 @@
     <t>Hypotheses and questions</t>
   </si>
   <si>
-    <t>Reading</t>
-  </si>
-  <si>
-    <t>Gotelli, N. J., &amp; Ellison, A. M. (2013) Chapter 4, "Framing and Testing Hypotheses", in A Primer of Ecological Statistics. Sinauer.</t>
-  </si>
-  <si>
-    <t>Course Book</t>
-  </si>
-  <si>
     <t>Data wrangling</t>
   </si>
   <si>
@@ -92,16 +80,7 @@
     <t>Pimping your plots</t>
   </si>
   <si>
-    <t>Broman, K. W., &amp; Woo, K. H. (2018). Data Organization in Spreadsheets. The American Statistician, 72(1), 2–10.; Wickham, H. (2014). Tidy Data. Journal of Statistical Software, 59(10), 1–23.</t>
-  </si>
-  <si>
-    <t>3 &amp; 4</t>
-  </si>
-  <si>
     <t>1 &amp; 2</t>
-  </si>
-  <si>
-    <t>The R graph gallery: https://www.r-graph-gallery.com/</t>
   </si>
   <si>
     <t>GSWR</t>
@@ -254,11 +233,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C11A616-6116-174C-ABC2-888311E75E63}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -585,953 +563,832 @@
     <col min="5" max="5" width="46.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F6">
         <v>3</v>
       </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F7">
         <v>3</v>
       </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
-      <c r="H8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12">
         <v>4</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12">
-        <v>5</v>
-      </c>
-      <c r="G12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F13">
-        <v>5</v>
-      </c>
-      <c r="G13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14">
         <v>4</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14">
-        <v>6</v>
-      </c>
-      <c r="G14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F15">
-        <v>6</v>
-      </c>
-      <c r="G15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F16">
-        <v>7</v>
-      </c>
-      <c r="G16">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F17">
-        <v>7</v>
-      </c>
-      <c r="G17">
         <v>8</v>
       </c>
-      <c r="H17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F22">
-        <v>9</v>
-      </c>
-      <c r="G22">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F24">
-        <v>10</v>
-      </c>
-      <c r="G24">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F26">
-        <v>11</v>
-      </c>
-      <c r="G26">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C27" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F28">
-        <v>12</v>
-      </c>
-      <c r="G28">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F32">
-        <v>14</v>
-      </c>
-      <c r="G32">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F33">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F34">
-        <v>15</v>
-      </c>
-      <c r="G34">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F35">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F37">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C44" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C45" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rebuikd with new schedule
</commit_message>
<xml_diff>
--- a/BB852_Schedule.xlsx
+++ b/BB852_Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jones/Dropbox/_SDU_Teaching/BB852/Course Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B37D95-1447-954D-B877-BECDE8219CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2268A731-0A32-C249-8CF4-5B803A6A38B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27220" yWindow="5280" windowWidth="28800" windowHeight="17500" xr2:uid="{CCA45BD5-8A90-4848-8BF8-FC958BC91D48}"/>
+    <workbookView xWindow="22400" yWindow="5280" windowWidth="28800" windowHeight="17500" xr2:uid="{CCA45BD5-8A90-4848-8BF8-FC958BC91D48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="51">
   <si>
     <t>Topic</t>
   </si>
@@ -545,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C11A616-6116-174C-ABC2-888311E75E63}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1356,13 +1356,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C44" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>38</v>
@@ -1373,15 +1373,66 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
         <v>41</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C48" t="s">
         <v>41</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rewrite for Autumn 2024
</commit_message>
<xml_diff>
--- a/BB852_Schedule.xlsx
+++ b/BB852_Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jones/GitHubRepos/BB852_Book/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA29C94-4AA0-9B45-8D0F-49CFCEA75329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4497C874-FE26-9549-AA5E-50F16C6CA984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{CCA45BD5-8A90-4848-8BF8-FC958BC91D48}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="60">
   <si>
     <t>Topic</t>
   </si>
@@ -122,12 +122,6 @@
     <t>Binomial GLMs in R</t>
   </si>
   <si>
-    <t>Mini Project</t>
-  </si>
-  <si>
-    <t>Project work</t>
-  </si>
-  <si>
     <t>Part</t>
   </si>
   <si>
@@ -194,14 +188,41 @@
     <t>Exam</t>
   </si>
   <si>
-    <t>Intro to Project Exam &amp; ChatGPT workshop</t>
+    <t>AI/ChatGPT workshop</t>
+  </si>
+  <si>
+    <t>Intro to Written Assignment</t>
+  </si>
+  <si>
+    <t>Written Assignment 2</t>
+  </si>
+  <si>
+    <t>Written Assignment 3</t>
+  </si>
+  <si>
+    <t>Written Assignment 4</t>
+  </si>
+  <si>
+    <t>Written Assignment 5</t>
+  </si>
+  <si>
+    <t>Written Assignment 6</t>
+  </si>
+  <si>
+    <t>Written Assignment 7</t>
+  </si>
+  <si>
+    <t>Written Assignment 8</t>
+  </si>
+  <si>
+    <t>Assignment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -214,6 +235,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -257,9 +284,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -297,7 +324,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -403,7 +430,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -545,7 +572,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -553,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C11A616-6116-174C-ABC2-888311E75E63}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,13 +594,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -582,7 +609,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G1" t="s">
         <v>15</v>
@@ -602,10 +629,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -625,7 +652,7 @@
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -642,10 +669,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
@@ -665,10 +692,10 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -691,7 +718,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -711,10 +738,10 @@
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G7">
         <v>3</v>
@@ -737,7 +764,7 @@
         <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -757,10 +784,10 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G9">
         <v>3</v>
@@ -780,10 +807,10 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -803,10 +830,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G11">
         <v>3</v>
@@ -826,10 +853,10 @@
         <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G12">
         <v>4</v>
@@ -849,10 +876,10 @@
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G13">
         <v>4</v>
@@ -875,7 +902,7 @@
         <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G14">
         <v>4</v>
@@ -895,10 +922,10 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G15">
         <v>4</v>
@@ -921,7 +948,7 @@
         <v>13</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G16">
         <v>8</v>
@@ -944,7 +971,7 @@
         <v>13</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G17">
         <v>8</v>
@@ -967,7 +994,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -987,7 +1014,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1004,10 +1031,10 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1024,10 +1051,10 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1047,7 +1074,7 @@
         <v>17</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G22">
         <v>5</v>
@@ -1067,10 +1094,10 @@
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1090,7 +1117,7 @@
         <v>18</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G24">
         <v>5</v>
@@ -1110,10 +1137,10 @@
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1133,7 +1160,7 @@
         <v>19</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G26">
         <v>5</v>
@@ -1156,7 +1183,7 @@
         <v>20</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1176,7 +1203,7 @@
         <v>21</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G28">
         <v>6</v>
@@ -1196,10 +1223,10 @@
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1219,7 +1246,7 @@
         <v>22</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1236,10 +1263,10 @@
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1259,7 +1286,7 @@
         <v>23</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G32">
         <v>7</v>
@@ -1279,10 +1306,10 @@
         <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1302,7 +1329,7 @@
         <v>24</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G34">
         <v>7</v>
@@ -1325,7 +1352,7 @@
         <v>27</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1345,7 +1372,7 @@
         <v>25</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1365,7 +1392,7 @@
         <v>26</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1376,16 +1403,16 @@
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D38" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1396,16 +1423,16 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D39" t="s">
         <v>2</v>
       </c>
       <c r="E39" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1416,16 +1443,16 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="D40" t="s">
         <v>2</v>
       </c>
       <c r="E40" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1436,16 +1463,16 @@
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="D41" t="s">
         <v>2</v>
       </c>
       <c r="E41" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1456,16 +1483,16 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="D42" t="s">
         <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1476,16 +1503,16 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="D43" t="s">
         <v>2</v>
       </c>
       <c r="E43" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1496,16 +1523,16 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D44" t="s">
         <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1516,19 +1543,100 @@
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D45" t="s">
         <v>2</v>
       </c>
       <c r="E45" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F45" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>23</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s">
+        <v>57</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>23</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>58</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>24</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s">
         <v>36</v>
       </c>
+      <c r="F48" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>24</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s">
+        <v>36</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>